<commit_message>
final working repository for preppoint (local testing unit) not production
</commit_message>
<xml_diff>
--- a/media/quiz/ecnomics_2015.xlsx
+++ b/media/quiz/ecnomics_2015.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="467">
   <si>
     <t>Question</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Answer</t>
   </si>
   <si>
     <t>Explanation</t>
@@ -50,7 +53,7 @@
 previous year</t>
   </si>
   <si>
-    <t>Microeconomics is a price theory, which studies the
+    <t>&lt;strong&gt;Microeconomics&lt;/strong&gt; is a price theory, which studies the
 economic behaviour of individual decision-making units,
 such as how the prices of resources levels or goods
 are determined. In contrast, macroeconomics studies
@@ -59,7 +62,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-The opportunity cost of any economic action is
+The&lt;strong&gt; opportunity cost&lt;/strong&gt; of any economic action is
 </t>
   </si>
   <si>
@@ -78,7 +81,7 @@
     <t>The next best alternative forgone</t>
   </si>
   <si>
-    <t>The production possibility curve (PPC) illustrates the
+    <t>&lt;strong&gt;The production possibility curve (PPC)&lt;/strong&gt; illustrates the
 concept of opportunity cost since the production of
 more of one good entail a sacrifice of the other. The
 sacrifice that is given up (or forgone) measures the
@@ -105,14 +108,14 @@
 </t>
   </si>
   <si>
-    <t>Shortage of economic resources mainly implies that
+    <t>⌂ &lt;strong&gt;Shortage of economic resources&lt;/strong&gt; mainly implies that
 people must compete to satisfy their wants. Since there
 is a shortage, those who pay the highest price may
-consume the good or service(commodity)
-There is an insufficient quantity of almost every
+consume the good or service(commodity)&lt;br&gt;
+⌂ There is an insufficient quantity of almost every
 commodity to satisfy all the wants of all members of
-society.
-Since resources are scarce, all the unlimited wants of
+society.&lt;br&gt;
+⌂ Since resources are scarce, all the unlimited wants of
 society can't be satisfied. Scarcity implies people must
 compete to satisfy their wants.</t>
   </si>
@@ -138,16 +141,16 @@
   </si>
   <si>
     <t xml:space="preserve">
-An entrepreneur is a person who undertakes, organizes,
+&lt;strong&gt;An Entrepreneur &lt;/strong&gt;is a person who undertakes, organizes,
 manages and assumes the risks of new enterprises or
-businesses.
+businesses.&lt;br&gt;
 So, the major role of entrepreneurs can play in an
 economy is taking risks to create businesses that yield
 products that meet the wants and needs of consumers.
 </t>
   </si>
   <si>
-    <t>The law of demand states that, ceteris paribus, the
+    <t>The &lt;strong&gt;Law of Demand &lt;/strong&gt;states that, ceteris paribus, the
 higher the price of a good,</t>
   </si>
   <si>
@@ -167,7 +170,7 @@
 </t>
   </si>
   <si>
-    <t>The law of demand states 'ceteris paribus" meaning the
+    <t>The law of demand states&lt;strong&gt; ''ceteris paribus"&lt;/strong&gt; meaning the
 higher the price of a good, the smaller is the quantity of
 the good demanded.</t>
   </si>
@@ -193,7 +196,7 @@
     <t>Rightward shift in the demand curve</t>
   </si>
   <si>
-    <t>&lt;img src="eco.jpg" &gt;</t>
+    <t>&lt;img class="quiz-image" src = "../media/quiz_images/economics_2013/demandcurve.jpg"&gt;</t>
   </si>
   <si>
     <t>Which of the following is a determinant of the demand
@@ -215,11 +218,10 @@
 </t>
   </si>
   <si>
-    <t>The determinants of demand for a good are:
-Own price of the good
-Income of the buyer (consumer)
-• Prices of related goods
-• Tastes and preferences, and so on.</t>
+    <t>&lt;strong&gt;The determinants of demand for a good are:&lt;/strong&gt;&lt;br&gt;
+⌂ Own price of the good Income of the buyer (consumer)&lt;br&gt;
+⌂ Prices of related goods&lt;br&gt;
+⌂ Tastes and preferences, and so on.&lt;br&gt;</t>
   </si>
   <si>
     <t>A Business College decides to increase tuition fees
@@ -276,7 +278,7 @@
   </si>
   <si>
     <t>If the cross-price elasticity of the demand for two
-products is -2.5, then the products are</t>
+products is &lt;strong&gt;-2.5&lt;/strong&gt;, then the products are</t>
   </si>
   <si>
     <t xml:space="preserve">Substitute and demand are cross price inelastic
@@ -325,12 +327,11 @@
     <t xml:space="preserve">For a rational consumer total utility is maximum when
 the marginal utility is zero. As the consumer continues
 to consume a commodity without any time gap, his or
-her utility, first increases, reaches a maximum when
-marginal utility is zero, and then declines.
-A rational consumer is one who:
-• has a clear-cut preference
-has a persistent preference
-• is subject to his/her budget constraints
+her utility, first increases, and reaches a maximum when
+marginal utility is zero and then declines.&lt;br&gt;
+⌂ &lt;strong&gt;A rational consumer is one who:&lt;/strong&gt;&lt;br&gt;
+• has a clear-cut preference has a persistent preference&lt;br&gt;
+• is subject to his/her budget constraints&lt;br&gt;
 </t>
   </si>
   <si>
@@ -354,8 +355,8 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Convexity of indifference curve shows that two goods
-can imperfectly substitute for one anothe.
+    <t xml:space="preserve">&lt;strong&gt;Convexity of indifference&lt;/strong&gt; curve shows that two goods
+can imperfectly substitute for one another.
 </t>
   </si>
   <si>
@@ -385,8 +386,8 @@
 inward.</t>
   </si>
   <si>
-    <t>In the ordinal theory of utility, the Income Consumption
-Curve (ICC) shows the way in which</t>
+    <t>In the ordinal theory of utility, &lt;strong&gt;the Income Consumption
+Curve (ICC) shows&lt;/strong&gt; the way in which</t>
   </si>
   <si>
     <t>Consumption varies as price of a commodity
@@ -410,7 +411,7 @@
 changes.</t>
   </si>
   <si>
-    <t>Which one of the following is true statement of a short
+    <t>Which one of the following is&lt;strong&gt; TRUE&lt;/strong&gt; statement of a short
 run production function with one variable input?</t>
   </si>
   <si>
@@ -432,13 +433,13 @@
   </si>
   <si>
     <t xml:space="preserve">Whenever the MP is greater than the AP the AP
-increases (Whenever MP &gt;AP =&gt; AP increases). This is
+increases &lt;strong&gt;(Whenever MP &gt;AP → AP increases).&lt;/strong&gt; This is
 true in a short-run production function with one variable
 input.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">The economic definition of market includes except
+    <t xml:space="preserve">The economic definition of market includes &lt;strong&gt;EXCEPT&lt;/strong&gt;
 </t>
   </si>
   <si>
@@ -458,39 +459,39 @@
 are able to exchange goods or services for money</t>
   </si>
   <si>
-    <t>A Market is a mechanism that brings buyers and sellers
+    <t>A &lt;strong&gt;Market&lt;/strong&gt; is a mechanism that brings buyers and sellers
 of a product together and interacts to exchange the
 product. It is not merely(only) limited to physical place it
 also includes online market (e-commerce).</t>
   </si>
   <si>
-    <t>In monopolistic competition firms maximize profit at the
+    <t>In &lt;strong&gt;Monopolistic competition&lt;/strong&gt; firms maximize profit at the
 level of output at which</t>
   </si>
   <si>
-    <t xml:space="preserve">Marginal revenue =Average revenue
+    <t xml:space="preserve">Marginal revenue = Average revenue
 </t>
   </si>
   <si>
-    <t>Marginal revenue=Marginal cost and marginal cost is
+    <t>Marginal revenue = Marginal cost and marginal cost is
 falling</t>
   </si>
   <si>
-    <t>Marginal revenue=Marginal cost and marginal cost is
+    <t>Marginal revenue = Marginal cost and marginal cost is
 rising</t>
   </si>
   <si>
-    <t xml:space="preserve">Marginal revenue=Average cost
+    <t xml:space="preserve">Marginal revenue = Average cost
 </t>
   </si>
   <si>
     <t>Profit maximization rule for firms, either in perfect
 competition, or monopolistic competition, or monopoly,
-or oligopoly is similar, i.e. MR = MC, and the MC is rising</t>
-  </si>
-  <si>
-    <t>Producers operating in monopolistically competitive
-markets are likely to</t>
+or oligopoly is similar, &lt;strong&gt;i.e. MR = MC, and the MC is rising&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Producers operating in&lt;strong&gt; Monopolistic competitive
+markets&lt;/strong&gt; are likely to</t>
   </si>
   <si>
     <t xml:space="preserve">Produce up to the point where marginal revenue is
@@ -512,13 +513,13 @@
   <si>
     <t xml:space="preserve">Firms in monopolistically competitive markets are likely
 to differentiate their products. One firm's product may
-be similar to another firm's product, but not identical.
-The product can be different from the other firm's
+be similar to another firm's product, but not identical.&lt;br&gt;
+⌂ The product can be different from the other firm's
 product in style, brand name, trademark, or in quality.
 </t>
   </si>
   <si>
-    <t>In a given society, which one is NOT considered as a cost
+    <t>In a given society, which one is&lt;strong&gt; NOT &lt;/strong&gt;considered as a cost
 of youth unemployment?</t>
   </si>
   <si>
@@ -538,7 +539,7 @@
 </t>
   </si>
   <si>
-    <t>A, B andC are considered to be the&lt;strong&gt; cost or the adverse
+    <t>&lt;strong&gt;A, B and C&lt;/strong&gt; are considered to be the&lt;strong&gt; cost or the adverse
 effect of youth unemployment &lt;/strong&gt;which implies giving
 power, skills or training to enable her/him to work
 efficiently and effectively, is a favorable effect.</t>
@@ -567,9 +568,9 @@
     <t>An increase in injections into the economy or increase
 in money supply in the economy may lead to an outward
 shift of the AD and demand-pull inflation. When the
-money supply increases, AD increases. When AD
+money supply increases, AD increases. &lt;br&gt;&lt;strong&gt;N.B: When AD
 increases general prices of goods increase, leading to
-demand-pull inflation.</t>
+demand-pull inflation.&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Which one of the following may give rise for a cost-push
@@ -592,15 +593,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">There are two types of inflation:
+    <t xml:space="preserve">There are two types of inflation:&lt;br&gt;
 • Demand-pull inflation is inflation of prices due to
 a shortage of supply compared to high demand. It
-is described as "too many dollars chasing too few
-goods". It is caused by a growing economy, government
-spending, rapid population growth. &lt;br&gt;Cost-push inflation is inflation that results from the
+is described as &lt;strong&gt;"too many dollars chasing too few
+goods"&lt;/strong&gt; It is caused by a growing economy, government
+spending, rapid population growth. &lt;br&gt;&lt;strong&gt;• Cost-push inflation &lt;/strong&gt; is inflation that results from the
 decrease in the supply of goods and services from an
 increase in the cost of production. An increase in the
-price of raw materials can cause cost-push inflation.
+price of raw materials can cause &lt;strong&gt;cost-push inflation.&lt;/strong&gt;
 </t>
   </si>
   <si>
@@ -628,8 +629,8 @@
   <si>
     <t xml:space="preserve">A devaluation of birr may cause inflation in the Ethiopian
 economy because it makes exports cheaper and
-imports expensive.
-This leads to inflation in the price of imported goods.
+imports expensive.&lt;br&gt;
+⌂ This leads to inflation in the price of imported goods.
 </t>
   </si>
   <si>
@@ -660,7 +661,7 @@
 highways, railways, airports, universities, hospitals, etc.</t>
   </si>
   <si>
-    <t>The primary use of national income accounting is to</t>
+    <t>The primary use of &lt;strong&gt;National Income Accounting&lt;/strong&gt; is to</t>
   </si>
   <si>
     <t>Asses the economic efficierncy of specific industries
@@ -683,7 +684,7 @@
 services produced in an economy in a year.</t>
   </si>
   <si>
-    <t>Which one of the following is fundamentally true?</t>
+    <t>Which one of the following is fundamentally&lt;strong&gt; TRUE&lt;/strong&gt;?</t>
   </si>
   <si>
     <t>Nominal GDP is always larger than real GDP</t>
@@ -698,11 +699,11 @@
     <t>Real GDP controls for changes in prices</t>
   </si>
   <si>
-    <t>Real GDP refers to GDP adjusted for inflation (price changes).</t>
-  </si>
-  <si>
-    <t>The difference between Gross National Product (GNP)
-and the Net National Product (NNP) is</t>
+    <t>Real &lt;strong&gt;GDP &lt;/strong&gt;refers to&lt;strong&gt; GDP&lt;/strong&gt; adjusted for inflation (price changes).</t>
+  </si>
+  <si>
+    <t>The difference between &lt;strong&gt;Gross National Product (GNP)&lt;/strong&gt;
+and the &lt;strong&gt;Net National Product (NNP)&lt;/strong&gt; is</t>
   </si>
   <si>
     <t>The net factor income from abroad</t>
@@ -718,11 +719,11 @@
     <t>Net taxes</t>
   </si>
   <si>
-    <t xml:space="preserve">NNP = GNP - Depreciation.
+    <t xml:space="preserve">&lt;strong&gt;NNP = GNP - Depreciation&lt;/strong&gt;
 </t>
   </si>
   <si>
-    <t>Which one of the following is NOT main property of
+    <t>Which one of the following is &lt;strong&gt;NOT&lt;/strong&gt; main property of
 Marginal Propensity to Consume (MPC)</t>
   </si>
   <si>
@@ -739,18 +740,14 @@
     <t>MPC is stable in the short-run</t>
   </si>
   <si>
-    <t>The Marginal Propensity to Consume (MPC) is the
-ratio of change in consumption(change in C) to change in
-income(change in Y).
-MPC= change in C/change in Y. The value of MPC is always between 0
-and 1.
-It is inversely proportional to a change in income.
-It doesn't rise with the increased income of the
-Consumers.</t>
-  </si>
-  <si>
-    <t>The sum of Marginal Propensity to Consume (MPC) and
-Marginal Propensity to Save (MPS) is always equal to</t>
+    <t>⌂ The&lt;strong&gt; Marginal Propensity to Consume (MPC)&lt;/strong&gt; is the ratio of change in consumption(change in C) to change in Income(change in Y).&lt;br&gt;
+⌂ MPC= change in C/change in Y. &lt;br&gt;⌂ The value of MPC is always between 0 and 1.&lt;br&gt;
+⌂ It is inversely proportional to a change in income.&lt;br&gt;
+⌂ It doesn't rise with the increased income of the Consumers.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>The &lt;strong&gt;sum of Marginal Propensity to Consume (MPC) and
+Marginal Propensity to Save (MPS)&lt;/strong&gt; is always equal to</t>
   </si>
   <si>
     <t>Unity</t>
@@ -769,7 +766,7 @@
     <t>MPC + MPS= ONE (unity)</t>
   </si>
   <si>
-    <t>International free trade is based on the principle of</t>
+    <t>&lt;strong&gt;International free trade&lt;/strong&gt; is based on the principle of</t>
   </si>
   <si>
     <t xml:space="preserve">Increasing economies of scale
@@ -786,10 +783,10 @@
     <t>Production possiblity advantage</t>
   </si>
   <si>
-    <t>International free trade is based on the principle of
-• Adam Smith's Theory of Absolute Cost Difference:
-Absolute Advantage
-David Ricardo's Theory of Comparative Cost:
+    <t>International free trade is based on the principle of&lt;br&gt;
+1) &lt;strong&gt;Adam Smith's Theory of Absolute Cost Difference:&lt;/strong&gt;
+Absolute Advantage&lt;br&gt;
+2) &lt;strong&gt;David Ricardo's Theory of Comparative Cost:&lt;/strong&gt;
 Comparative Advantage</t>
   </si>
   <si>
@@ -809,10 +806,10 @@
     <t>Trade balance</t>
   </si>
   <si>
-    <t>When exports &gt; imports, the country is said to have a
-trade surplus.
-• When exports &lt; imports, the country is said to have a
-trade deficit.</t>
+    <t>⌂ When exports &gt; imports, the country is said to have a
+&lt;strong&gt;trade surplus.&lt;/strong&gt;&lt;br&gt;
+⌂ When exports &lt; imports, the country is said to have a
+&lt;strong&gt;trade deficit.&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Balance of trade commonly refers to</t>
@@ -835,7 +832,7 @@
 payment made for imports in a year</t>
   </si>
   <si>
-    <t>A Trade balance is merchandise exports minus
+    <t>&lt;strong&gt;Trade balance&lt;/strong&gt; is merchandise exports minus
 merchandise imports.</t>
   </si>
   <si>
@@ -860,11 +857,11 @@
 eliminate the excess supply</t>
   </si>
   <si>
-    <t>In a fixed exchange rate:
-When there is an excess demand of foreign exchange,
+    <t>&lt;strong&gt;In a fixed exchange rate:&lt;/strong&gt;&lt;br&gt;
+•  When there is an excess demand of foreign exchange,
 the central bank of the country has to sell foreign
-exchange to eliminate excess demand.
-•When there is an excess supply of foreign exchange,
+exchange to eliminate excess demand.&lt;br&gt;
+• When there is an excess supply of foreign exchange,
 the central bank of the country has to buy foreign
 exchange to eliminate the excess supply.</t>
   </si>
@@ -885,12 +882,12 @@
     <t>Supply and the exchange rate should rise</t>
   </si>
   <si>
-    <t>A Floating exchange rate is based on the supply and
-demand relative to other countries.
-In a floating exchange rate:
+    <t>&lt;strong&gt;Floating exchange rate&lt;/strong&gt; is based on the supply and
+demand relative to other countries.&lt;br&gt;
+&lt;strong&gt;In a floating exchange rate:&lt;/strong&gt;&lt;br&gt;
 • if the exchange rate is above the equilibrium level,
 there is excess supply and the exchange rate should
-fall.
+fall.&lt;br&gt;
 • if the exchange rate is below the equilibrium level,
 there is excess demand and the exchange rate should
 rise.</t>
@@ -919,7 +916,7 @@
 and services.</t>
   </si>
   <si>
-    <t>Which one of the following is NOT an instrument of
+    <t>Which one of the following is &lt;strong&gt;NOT&lt;/strong&gt; an instrument of
 expansionary monetary policy?</t>
   </si>
   <si>
@@ -947,7 +944,7 @@
 is about</t>
   </si>
   <si>
-    <t>Mining contributes only 1% to Ethiopia's GDP. Gold,
+    <t>⌂ Mining contributes only 1% to Ethiopia's GDP. &lt;br&gt;⌂ Gold,
 marble, limestone and tantalum are the major minerals
 mined in Ethiopia.</t>
   </si>
@@ -968,11 +965,11 @@
     <t>40 years</t>
   </si>
   <si>
-    <t>Median is the middle of a sorted list of numbers. The median age of Ethiopia is around is around 20 years old.</t>
+    <t>&lt;strong&gt;Median&lt;/strong&gt; is the middle of a sorted list of numbers. The median age of Ethiopia is around is around 20 years old.</t>
   </si>
   <si>
     <t>Ethiopia has ratified the following international
-agreement on environment except</t>
+agreement on environment &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Ozone Layer protection</t>
@@ -988,7 +985,7 @@
   </si>
   <si>
     <t>Concerning environmental protection, Ethiopia has not
-ratified the "law of the sea' agreement.</t>
+ratified the &lt;strong&gt;"law of the sea"&lt;/strong&gt; agreement.</t>
   </si>
   <si>
     <t>Under the Derg regime, the following National
@@ -1008,7 +1005,7 @@
     <t>Peace, Democracy and Development Programs</t>
   </si>
   <si>
-    <t>Peace, Democracy and Development programs are the
+    <t>&lt;strong&gt;Peace, Democracy and Development programs&lt;/strong&gt; are the
 National Development Plan of the EPRDF government,
 during 1992 -1996.</t>
   </si>
@@ -1036,7 +1033,7 @@
 GTPI, followed by PASDEP.</t>
   </si>
   <si>
-    <t>The following are true of Bi-modal agricultural strategy
+    <t>The following are &lt;strong&gt;TRUE&lt;/strong&gt; of Bi-modal agricultural strategy
 except it</t>
   </si>
   <si>
@@ -1052,11 +1049,11 @@
     <t>Allows the transfer of technology</t>
   </si>
   <si>
-    <t>Lack off-farm job opportunities is one of the limitations
+    <t>&lt;strong&gt;Lack off-farm job opportunities&lt;/strong&gt; is one of the limitations
 Bi-modal agricultural strategy.</t>
   </si>
   <si>
-    <t>Which of the following is not true about the agriculture
+    <t>Which of the following is &lt;strong&gt;NOT TRUE&lt;/strong&gt; about the agriculture
 sector in Ethiopia</t>
   </si>
   <si>
@@ -1077,8 +1074,8 @@
 contributed the largest share in in Ethiopia's GDP.</t>
   </si>
   <si>
-    <t>challenges in an attempt to transform the Ethiopian
-agricultural sector include except</t>
+    <t>Challenges in an attempt to transform the Ethiopian
+agricultural sector include &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Inappropriate pricing policy towards agricultural land
@@ -1102,7 +1099,7 @@
   <si>
     <t>To mitigate the problems affecting the Ethiopian
 agricultural sector, it is important to take the following
-possible remedies except</t>
+possible remedies &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Reduces the prevailing heavy dependence on rain-fed
@@ -1121,7 +1118,7 @@
     <t>Use capital intensive technology.</t>
   </si>
   <si>
-    <t>Capital intensive technology is a technology that
+    <t>&lt;strong&gt;Capital intensive technology&lt;/strong&gt; is a technology that
 requires a very large amount of investment. Since
 Ethiopia is a developing country, using capital-intensive
 technology can affect the country's economy. It can't be
@@ -1161,7 +1158,7 @@
   </si>
   <si>
     <t>The Ethiopian industrial sector is characterized by the
-following except</t>
+following &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Absence of adequate institutional support</t>
@@ -1176,7 +1173,7 @@
     <t>Usage of labor-intensive technology.</t>
   </si>
   <si>
-    <t>The Ethiopian industrial sector is not characterized
+    <t>The&lt;strong&gt; Ethiopian industrial sector&lt;/strong&gt; is not characterized
 by the usage of labor-intensive technology. It is rather
 characterized by the usage of capital-intensive
 technology.</t>
@@ -1205,7 +1202,7 @@
 manufacturing hub within Africa.</t>
   </si>
   <si>
-    <t>The theory of linkages stresses that</t>
+    <t>The &lt;strong&gt;theory of linkages&lt;/strong&gt; stresses that</t>
   </si>
   <si>
     <t>When certain industries are developed first, their
@@ -1227,9 +1224,8 @@
 sector is very strong in developing countries.</t>
   </si>
   <si>
-    <t>Theory of Linkages states when certain industries
-are developed, it promotes the interconnection and
-development of other industries.</t>
+    <t>&lt;strong&gt;Theory of Linkages&lt;strong&gt; states&lt;br&gt; &lt;i&gt;"When certain industries
+are developed, it promotes the interconnection and development of other industries."&lt;/i&gt;</t>
   </si>
   <si>
     <t>In an industry when a firm buys a good from another firm
@@ -1266,8 +1262,7 @@
 together in cities and industrial clusters resulting in cost
 reduction.&lt;br&gt;
 &lt;strong&gt;• Localization economies&lt;/strong&gt; occur when an increase in the
-size of an industry in a city leads to an increase in the
-productivity of a particular activity.</t>
+size of an industry in a city leads to an increase in the productivity of a particular activity.</t>
   </si>
   <si>
     <t>Two major service providers that help Ethiopia earn
@@ -1295,7 +1290,7 @@
   </si>
   <si>
     <t>The 1992 proclamation on Ethiopian transport policy
-allows except</t>
+allows &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Regulation of the freight transport industry.</t>
@@ -1338,7 +1333,7 @@
 from African countries.</t>
   </si>
   <si>
-    <t>All are key resource bases of Ethiopia except</t>
+    <t>All are key resource bases of Ethiopia &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Abundant valuable minerals.</t>
@@ -1379,7 +1374,7 @@
 (close to 50%)</t>
   </si>
   <si>
-    <t>ldentify the correct statement about minerals and
+    <t>ldentify the &lt;strong&gt;CORRECT&lt;/strong&gt; statement about minerals and
 environment in Ethiopia.</t>
   </si>
   <si>
@@ -1492,7 +1487,7 @@
   </si>
   <si>
     <t>Concerning the agriculture sector of Ethiopia, all are the
-major challenges except</t>
+major challenges &lt;strong&gt;EXCEPT&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Lack of fertile land</t>
@@ -1513,7 +1508,7 @@
   </si>
   <si>
     <t>From the under-listed policy interventions, the one which
-does not enhance agricultural productivity in Ethiopia is__________</t>
+does not enhance agricultural productivity in Ethiopia is __________</t>
   </si>
   <si>
     <t>Introduction of new and improved varieties of seeds
@@ -1632,19 +1627,19 @@
 negligible.</t>
   </si>
   <si>
-    <t>Ethiopia Industrial Sector may lead to superior
-outcomes because:
+    <t>&lt;strong&gt; Ethiopia Industrial Sector may lead to superior
+outcomes because:&lt;/strong&gt;&lt;br&gt;
 • it is directed to use local raw materials, which creates
-strong linkages with other sectors.
+strong linkages with other sectors.&lt;br&gt;
 • it has a high potential to create job opportunities
-rapidly in urban areas.
-•A developed industrial sector generates more foreign
+rapidly in urban areas.&lt;br&gt;
+• a developed industrial sector generates more foreign
 currency compared to other sectors</t>
   </si>
   <si>
     <t>Suppose Mugher cement factory has decided to
 subcontract supply of some inputs (e.g., limestone)
-to local farmers who own the minerals. this type of
+to local farmers who own the minerals. &lt;br&gt;This type of
 linkage between an industry and inputs supplies is called__________</t>
   </si>
   <si>
@@ -1662,7 +1657,7 @@
 Consumption linkages</t>
   </si>
   <si>
-    <t>Forward linkages refer to the part of the non-farm sector
+    <t>&lt;strong&gt;Forward linkages&lt;/strong&gt; refer to the part of the non-farm sector
 that uses agricultural output as an input.
 In this case, the cement factory (non-farm) sector uses
 (limestone) agricultural output as an input.</t>
@@ -1682,10 +1677,10 @@
     <t>Infrastructure linkages</t>
   </si>
   <si>
-    <t>According &lt;strong&gt;Hirschmann:&lt;/strong&gt;&lt;br&gt;&lt;strong&gt; forward linkage&lt;/strong&gt; is created when investment in a
+    <t>According &lt;strong&gt;Hirschmann:&lt;/strong&gt;&lt;br&gt;⌂ &lt;strong&gt; Forward linkage&lt;/strong&gt; is created when investment in a
 particular project encourages investment in subsequent
 stages of production.&lt;br&gt;
-&lt;strong&gt;backward linkage&lt;/strong&gt; is created when a project
+⌂ &lt;strong&gt;Backward linkage&lt;/strong&gt; is created when a project
 encourages investment in facilities that enable the
 project to succeed.&lt;br&gt;</t>
   </si>
@@ -1709,11 +1704,11 @@
     <t>Very low and insignificant and hence can be ignored</t>
   </si>
   <si>
-    <t>In the 2008/9 GC, Ethiopia's foreign exchange income
-from:
+    <t>&lt;strong&gt;In the 2008/9 GC, Ethiopia's foreign exchange income
+from:&lt;/strong&gt;&lt;br&gt;
 • The merchandise export was 1.45 billion Dollar.
 The service sector mainly from Ethiopia Airlines and
-Ethiopian was 2 billion Dollar.
+Ethiopian was 2 billion Dollar.&lt;br&gt;
 • The manufacturing sector was 700million dollar.
 So, the foreign exchange income from the Service
 Sector in Ethiopia was better than the merchandise
@@ -1747,12 +1742,13 @@
 marginal product of the ninth worker equals___________</t>
   </si>
   <si>
-    <t>&lt;img src="z_desc_71.jpg" &gt;</t>
-  </si>
-  <si>
-    <t>A firm's total cost function is given by: TC=300-6Q+4Q2
+    <t xml:space="preserve">
+&lt;img class="quiz-image" src = "../media/quiz_images/economics_2013/marginalproduct.jpg"&gt;</t>
+  </si>
+  <si>
+    <t>A firm's total cost function is given by: &lt;strong&gt;TC = 300 - 6Q + 4Q2&lt;/strong&gt;
 where TC refers to total cost in birr and Q refers to
-quantity produced in kilograms. When Q=4, the marginal
+quantity produced in kilograms. When Q = 4, the marginal
 and average variable costs are</t>
   </si>
   <si>
@@ -1768,9 +1764,9 @@
     <t>12 and 16 birr per kilogram respectively</t>
   </si>
   <si>
-    <t>MC = 26 and AVC= 10
-MC = -6 + 8Q → -6+ (8x4) = -6 + 32 = 26
-AVC = -6 + 4Q -6 + (4x4) = -6+ 16 = 10</t>
+    <t>MC = 26 and AVC = 10&lt;br&gt;
+MC = -6 + 8Q → -6 + (8 x 4) = -6 + 32 = 26&lt;br&gt;
+AVC = -6 + 4Q → -6 + (4 x 4) = -6+ 16 = 10</t>
   </si>
   <si>
     <t>Assume firm's total cost of producing 8 units of output
@@ -1790,17 +1786,21 @@
     <t>4 birr per units</t>
   </si>
   <si>
-    <t>AC= TC/Q → 160/8 = 20birr
-AC= AVC + AFC
-Birr 20 = AVC + 2 Birr
-AVC = 20-2 = 18 Birr per units</t>
+    <t>AC = TC/Q → 160/8 = 20birr&lt;br&gt;
+AC = AVC + AFC&lt;br&gt;
+Birr 20 = AVC + 2 Birr&lt;br&gt;
+&lt;strong&gt;AVC = 20-2 = 18 Birr per units&lt;/strong&gt;</t>
   </si>
   <si>
     <t>Consider the following short run production function
 where capital is assumed to be constant and answer
-questions of 74 and 75. Q=8L2 -0.2L3 where Q refers
+questions of 74 and 75. &lt;strong&gt;Q=8L² - 0.2L³&lt;/strong&gt; where Q refers
 to output and L refers to labor. The value of labor that
-maximizes average product is________________</t>
+maximizes average product is________________.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;img class="quiz-image" src = "../media/quiz_images/economics_2013/averageproduct.jpg"&gt;</t>
   </si>
   <si>
     <t>Consider the following short run production function
@@ -1810,20 +1810,20 @@
 labor that maximizes marginal product is______________</t>
   </si>
   <si>
-    <t>The value of labor that maximizes marginal product is
-the derivate of marginal product.
+    <t>&lt;strong&gt;The value of labor that maximizes marginal product is
+the derivate of marginal product.&lt;/strong&gt;&lt;br&gt;
 &lt;strong&gt;Step 1&lt;/strong&gt;&lt;br&gt;
-Let's first get the marginal product (MP)
-MP = dQ/dL = 16L- 0.6L2
-Step 2
-Let's now gets the max. marginal product
-dMp/dL= 16 - 1.2L = 0
-1.2L = 16
-L= 13.33'
-L~ 13</t>
-  </si>
-  <si>
-    <t>Which one of the following relationships holds true?</t>
+⌂ Let's first get the marginal product (MP)&lt;br&gt;
+MP = dQ/dL = 16L- 0.6L²&lt;br&gt;
+&lt;strong&gt;Step 2&lt;/strong&gt;&lt;br&gt;
+⌂ Let's now gets the max. marginal product&lt;br&gt;
+dMp / dL = 16 - 1.2L = 0&lt;br&gt;
+1.2L = 16&lt;br&gt;
+L= 13.33'&lt;br&gt;
+&lt;strong&gt;L≈ 13&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Which one of the following relationships holds &lt;strong&gt;TRUE?&lt;/strong&gt;</t>
   </si>
   <si>
     <t>When marginal product is rising, marginal cost of
@@ -1842,11 +1842,11 @@
 marginal cost of labor is at its falling.</t>
   </si>
   <si>
-    <t>The MC (Marginal Cost) curve is a mirror image or
-reciprocal of the MPL (Marginal Product Labor) curve.
-When the MPL curve rises, MC curve falls;
-• when the MPL is maximum, the MC is minimum;
-• when MPL falls, the MC rises.</t>
+    <t>The &lt;strong&gt;MC (Marginal Cost) curve&lt;/strong&gt; is a mirror image or
+reciprocal of the MPL (Marginal Product Labor) curve.&lt;br&gt;
+• When the MPL curve rises, MC curve falls;&lt;br&gt;
+• When the MPL is maximum, the MC is minimum;&lt;br&gt;
+• When MPL falls, the MC rises.</t>
   </si>
   <si>
     <t>To prevent a firm shutting down in the short run, it must</t>
@@ -1864,13 +1864,13 @@
     <t>Cover both fixed and variable costs.</t>
   </si>
   <si>
-    <t>The shutdown rule states that a firm should continue
+    <t>&lt;strong&gt;shutdown rule states&lt;/strong&gt;&lt;br&gt;&lt;i&gt;"a firm should continue
 operations as long as it can cover variable costs. In the
-short run, fixed costs are not considered.</t>
-  </si>
-  <si>
-    <t>Which one of the following is true on the relationship
-between the average and marginal costs in short-run?</t>
+short run, fixed costs are not considered."&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Which one of the following is &lt;strong&gt;true&lt;/strong&gt; in the relationship
+between the average and marginal costs in the short-run?</t>
   </si>
   <si>
     <t>Whenever marginal cost lies below average variable
@@ -1897,7 +1897,7 @@
     <t>Assume a German tourist visits an obelisk in Axum city:
 and hires a local taxi, rent a room for a couple of days
 in Ezana hotel, and eats meals in this hotel. Given this
-statement, which one of the following is not true?</t>
+statement, which one of the following is &lt;strong&gt;NOT TRUE&lt;/strong&gt;?</t>
   </si>
   <si>
     <t>The goods and services consumed by the German
@@ -1916,23 +1916,23 @@
 tourist are counted as part of Germany's GNP</t>
   </si>
   <si>
-    <t>Gross Domestic Product (GDP) is the total value of
+    <t>•  &lt;strong&gt;Gross Domestic Product (GDP)&lt;/strong&gt; is the total value of
 the goods and services produced within a country's
-borders.
+borders.&lt;br&gt;
 • GDP = Consumption + Investment + Government +
-Exports - Imports
-Gross National Product (GNP) is the total value of the
+Exports - Imports&lt;br&gt;
+• &lt;strong&gt;Gross National Product (GNP)&lt;/strong&gt; is the total value of the
 goods and services produced by the residents of a
-country, no matter their location.
-GNP = GDP + Net Income by citizens from a foreign
-country - Net Income by foreigners in the country
-The goods and services consumed by the Gernman
-tourists are counted as Germany GNP, Ethiopia GDP and
-Ethiopia GNP. It is not considered as export items.</t>
+country, no matter their location.&lt;br&gt;
+• &lt;strong&gt;GNP = GDP + Net Income by citizens from a foreign
+country - Net Income by foreigners in the country&lt;/strong&gt;&lt;br&gt;
+• The goods and services consumed by the German
+tourists are counted as Germany's GNP, Ethiopia's GDP and
+Ethiopia GNP. It is not considered an export item.</t>
   </si>
   <si>
     <t>To fight inflation, government or the central bank should
-NOT do one of the following</t>
+&lt;strong&gt;NOT&lt;/strong&gt; do one of the following</t>
   </si>
   <si>
     <t>Increasing discount interest rate</t>
@@ -2231,9 +2231,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -2258,25 +2260,25 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2301,25 +2303,25 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2344,25 +2346,25 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2387,25 +2389,25 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2430,25 +2432,25 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2473,25 +2475,25 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2516,25 +2518,25 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2559,25 +2561,25 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2602,25 +2604,25 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2645,25 +2647,25 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2688,25 +2690,25 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2731,25 +2733,25 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2774,25 +2776,25 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2817,23 +2819,25 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G15" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2858,25 +2862,25 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2901,25 +2905,25 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -2944,25 +2948,25 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2987,25 +2991,25 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -3030,25 +3034,25 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3073,25 +3077,25 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3116,25 +3120,25 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3159,25 +3163,25 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3202,25 +3206,25 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3245,25 +3249,25 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -3288,25 +3292,25 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -3331,25 +3335,25 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -3374,25 +3378,25 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -3417,25 +3421,25 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -3460,25 +3464,25 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -3503,25 +3507,25 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -3546,25 +3550,25 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -3589,25 +3593,25 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -3632,25 +3636,25 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -3675,25 +3679,25 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -3718,25 +3722,25 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -3761,7 +3765,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B37" s="3">
         <v>0.01</v>
@@ -3779,7 +3783,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -3804,25 +3808,25 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -3847,25 +3851,25 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -3890,25 +3894,25 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -3933,25 +3937,25 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -3976,25 +3980,25 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -4019,25 +4023,25 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -4062,25 +4066,25 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -4105,25 +4109,25 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -4148,25 +4152,25 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -4191,25 +4195,25 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -4234,25 +4238,25 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -4277,25 +4281,25 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -4320,25 +4324,25 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -4363,25 +4367,25 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -4406,25 +4410,25 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -4449,25 +4453,25 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -4492,25 +4496,25 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -4535,25 +4539,25 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -4578,25 +4582,25 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -4621,25 +4625,25 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -4664,25 +4668,25 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -4707,25 +4711,25 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -4750,25 +4754,25 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -4793,25 +4797,25 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -4836,25 +4840,25 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -4879,25 +4883,25 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -4922,25 +4926,25 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -4965,25 +4969,25 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -5008,25 +5012,25 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -5051,25 +5055,25 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -5094,25 +5098,25 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -5137,25 +5141,25 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -5180,25 +5184,25 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -5223,25 +5227,25 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -5266,7 +5270,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B72" s="1">
         <v>804.0</v>
@@ -5284,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -5309,25 +5313,25 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -5352,25 +5356,25 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -5395,7 +5399,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B75" s="1">
         <v>20.0</v>
@@ -5412,7 +5416,9 @@
       <c r="F75" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G75" s="2"/>
+      <c r="G75" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
@@ -5436,7 +5442,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B76" s="1">
         <v>10.0</v>
@@ -5454,7 +5460,7 @@
         <v>2</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -5479,25 +5485,25 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -5522,25 +5528,25 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -5565,25 +5571,25 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -5608,25 +5614,25 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -5651,25 +5657,25 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>

</xml_diff>